<commit_message>
working code with bug fix. Implement oop
</commit_message>
<xml_diff>
--- a/RunManager.xlsx
+++ b/RunManager.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Full suite" sheetId="1" r:id="rId1"/>
+    <sheet name="d" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -19,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="11">
-  <si>
-    <t>Test Scenario</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="22">
   <si>
     <t>TestCase_ID</t>
   </si>
@@ -36,22 +34,58 @@
     <t>No</t>
   </si>
   <si>
-    <t>Sprint 1</t>
-  </si>
-  <si>
-    <t>Sprint 1_LogIn</t>
-  </si>
-  <si>
     <t>Sprint 1_Create Payment</t>
   </si>
   <si>
-    <t>Sprint 2</t>
-  </si>
-  <si>
-    <t>Test for log in with valid credential</t>
-  </si>
-  <si>
     <t>Create payment</t>
+  </si>
+  <si>
+    <t>Sprint 1_Log in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abc </t>
+  </si>
+  <si>
+    <t>uio</t>
+  </si>
+  <si>
+    <t>lko</t>
+  </si>
+  <si>
+    <t>sas</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>rt</t>
+  </si>
+  <si>
+    <t>ioio</t>
+  </si>
+  <si>
+    <t>ioioiioioioi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log in </t>
+  </si>
+  <si>
+    <t>Sprint 1_Create rttrt</t>
+  </si>
+  <si>
+    <t>Sprint 1_Create uyuyu</t>
+  </si>
+  <si>
+    <t>Sprint 1_Create kjkjk</t>
+  </si>
+  <si>
+    <t>Sprint 1_Create 787878</t>
+  </si>
+  <si>
+    <t>Sprint 1_Log out</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -88,7 +122,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -111,11 +145,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -124,6 +171,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -440,21 +490,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="47.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -464,253 +513,281 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
       <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
       <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
       <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
       <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
       <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
       <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
       <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
       <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
       <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
       <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
       <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
       <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
       <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
       <c r="B20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
       <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C21">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>